<commit_message>
Fixed disciplinary info on all 2016 CRS home games
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-crs-fckc-073016.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-crs-fckc-073016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/push/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1455"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A1264" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="S1270" sqref="S1270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>